<commit_message>
Issues status is updated
</commit_message>
<xml_diff>
--- a/Retinue To Do.xlsx
+++ b/Retinue To Do.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,12 @@
     <sheet name="Feature" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="36">
   <si>
     <t>No</t>
   </si>
@@ -115,13 +115,22 @@
   </si>
   <si>
     <t>Very Important</t>
+  </si>
+  <si>
+    <t>Vanilla.Accontat.Facade.Invoice.LineItem.Server.cs -&gt; public override BinAff.Facade.Library.Dto Convert(BinAff.Core.Data data) has thrown object reference not set to an reference error while loading old record</t>
+  </si>
+  <si>
+    <t>Check in</t>
+  </si>
+  <si>
+    <t>Opne</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -262,7 +271,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -297,7 +305,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -473,14 +480,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.42578125" style="5" customWidth="1"/>
@@ -490,7 +497,7 @@
     <col min="7" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -510,7 +517,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="30">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -521,10 +528,10 @@
         <v>23</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -538,7 +545,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="30">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -552,7 +559,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -566,7 +573,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -580,7 +587,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="30">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -597,7 +604,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="30">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -611,7 +618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="45">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -626,6 +633,20 @@
       </c>
       <c r="F9" s="3" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45">
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -634,14 +655,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="71.42578125" customWidth="1"/>
@@ -649,7 +670,7 @@
     <col min="6" max="6" width="62.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,7 +690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -683,7 +704,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -697,7 +718,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -711,7 +732,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -722,7 +743,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -736,7 +757,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -750,7 +771,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -764,7 +785,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -785,12 +806,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>